<commit_message>
fin de jounee 06 11 image update + bouton
</commit_message>
<xml_diff>
--- a/DOC/PBN_JDB.xlsx
+++ b/DOC/PBN_JDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
   <si>
     <t>Date</t>
   </si>
@@ -289,6 +289,24 @@
   </si>
   <si>
     <t>Inegration du log la semain prochaine si possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information générale parraport au stage et le deroulement de la sem. com M. Chevillat </t>
+  </si>
+  <si>
+    <t>Implémenté la fonctionalité "Preview" pour les images</t>
+  </si>
+  <si>
+    <t>Débugger le chargement de l'image en applicant une nouvelle logique</t>
+  </si>
+  <si>
+    <t>Chercher intensive sur le net pour comprendre pourquoi le chargement retourne une erreur qui fait crasher le logiciel</t>
+  </si>
+  <si>
+    <t>Rendre fonctionels les deux boutons dédié à l'ouverture de fichier</t>
+  </si>
+  <si>
+    <t>Insertion d'une securité niveau code au cas où l'image "Preview" n'arrive pas à étre chargée</t>
   </si>
 </sst>
 </file>
@@ -648,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -748,6 +766,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -757,8 +778,74 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -766,74 +853,27 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,26 +1187,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="18"/>
+    <col min="1" max="1" width="13.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="3" max="3" width="79" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
     <col min="5" max="5" width="55" customWidth="1"/>
     <col min="6" max="6" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="64"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1175,9 +1215,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="63"/>
+      <c r="A2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1224,12 +1264,12 @@
         <f>SUM(B8:B13)</f>
         <v>0.10069444444444445</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="56"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="59"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="49">
+      <c r="A8" s="68">
         <v>43343</v>
       </c>
       <c r="B8" s="27">
@@ -1242,7 +1282,7 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="21">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1255,7 +1295,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="69"/>
       <c r="B10" s="20">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1266,7 +1306,7 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="20">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1277,7 +1317,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="20">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1288,7 +1328,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="17">
         <v>3.125E-2</v>
       </c>
@@ -1306,14 +1346,14 @@
         <f>SUM(B15:B23)</f>
         <v>0.1875</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="59"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49">
+      <c r="A15" s="68">
         <v>43347</v>
       </c>
       <c r="B15" s="25">
@@ -1328,7 +1368,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="20">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1340,7 +1380,7 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="20">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1352,7 +1392,7 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
+      <c r="A18" s="69"/>
       <c r="B18" s="20">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1365,7 +1405,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="50">
+      <c r="A19" s="69">
         <v>43350</v>
       </c>
       <c r="B19" s="25">
@@ -1378,7 +1418,7 @@
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
+      <c r="A20" s="69"/>
       <c r="B20" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1391,7 +1431,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
+      <c r="A21" s="69"/>
       <c r="B21" s="25">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1402,7 +1442,7 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="69"/>
       <c r="B22" s="25">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1413,7 +1453,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47"/>
+      <c r="A23" s="70"/>
       <c r="B23" s="20">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1431,14 +1471,14 @@
         <f>SUM(B25:B34)</f>
         <v>0.1875</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="49">
+      <c r="A25" s="68">
         <v>43354</v>
       </c>
       <c r="B25" s="21">
@@ -1453,7 +1493,7 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
+      <c r="A26" s="69"/>
       <c r="B26" s="21">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1466,7 +1506,7 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1474,14 +1514,14 @@
         <v>35</v>
       </c>
       <c r="D27" s="16"/>
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="73" t="s">
         <v>36</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
+      <c r="A28" s="69"/>
       <c r="B28" s="21">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1489,10 +1529,10 @@
         <v>37</v>
       </c>
       <c r="D28" s="16"/>
-      <c r="E28" s="51"/>
+      <c r="E28" s="73"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
+      <c r="A29" s="69"/>
       <c r="B29" s="21">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1500,11 +1540,11 @@
         <v>73</v>
       </c>
       <c r="D29" s="16"/>
-      <c r="E29" s="51"/>
+      <c r="E29" s="73"/>
       <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50">
+      <c r="A30" s="69">
         <v>43357</v>
       </c>
       <c r="B30" s="21">
@@ -1517,7 +1557,7 @@
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
+      <c r="A31" s="69"/>
       <c r="B31" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1525,12 +1565,12 @@
         <v>39</v>
       </c>
       <c r="D31" s="16"/>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="73" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
+      <c r="A32" s="69"/>
       <c r="B32" s="21">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1538,10 +1578,10 @@
         <v>41</v>
       </c>
       <c r="D32" s="15"/>
-      <c r="E32" s="51"/>
+      <c r="E32" s="73"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
+      <c r="A33" s="69"/>
       <c r="B33" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1549,10 +1589,10 @@
         <v>42</v>
       </c>
       <c r="D33" s="15"/>
-      <c r="E33" s="51"/>
+      <c r="E33" s="73"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="47"/>
+      <c r="A34" s="70"/>
       <c r="B34" s="21">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1566,14 +1606,14 @@
       <c r="A35" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="52" t="s">
+      <c r="C35" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="52"/>
-      <c r="E35" s="53"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="61"/>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
@@ -1583,12 +1623,12 @@
         <f>SUM(B37:B47)</f>
         <v>0.1875</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="59"/>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="49">
+      <c r="A37" s="68">
         <v>43368</v>
       </c>
       <c r="B37" s="21">
@@ -1605,7 +1645,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
+      <c r="A38" s="69"/>
       <c r="B38" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1616,7 +1656,7 @@
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
+      <c r="A39" s="69"/>
       <c r="B39" s="21">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1629,7 +1669,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="50"/>
+      <c r="A40" s="69"/>
       <c r="B40" s="21">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1640,7 +1680,7 @@
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
+      <c r="A41" s="69"/>
       <c r="B41" s="21">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1651,7 +1691,7 @@
       <c r="E41" s="13"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="50">
+      <c r="A42" s="69">
         <v>43371</v>
       </c>
       <c r="B42" s="21">
@@ -1664,7 +1704,7 @@
       <c r="E42" s="13"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
+      <c r="A43" s="69"/>
       <c r="B43" s="21">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1677,7 +1717,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="50"/>
+      <c r="A44" s="69"/>
       <c r="B44" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1688,7 +1728,7 @@
       <c r="E44" s="13"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
+      <c r="A45" s="69"/>
       <c r="B45" s="21">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1699,7 +1739,7 @@
       <c r="E45" s="13"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
+      <c r="A46" s="69"/>
       <c r="B46" s="21">
         <v>1.7361111111111112E-2</v>
       </c>
@@ -1710,7 +1750,7 @@
       <c r="E46" s="13"/>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="47"/>
+      <c r="A47" s="70"/>
       <c r="B47" s="30">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1728,12 +1768,12 @@
         <f>SUM(B49:B60)</f>
         <v>9.3750000000000014E-2</v>
       </c>
-      <c r="C48" s="54"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="56"/>
+      <c r="C48" s="57"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="59"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="48">
+      <c r="A49" s="71">
         <v>43375</v>
       </c>
       <c r="B49" s="21">
@@ -1748,7 +1788,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="48"/>
+      <c r="A50" s="71"/>
       <c r="B50" s="21">
         <v>2.4305555555555556E-2</v>
       </c>
@@ -1761,7 +1801,7 @@
       <c r="E50" s="13"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="48"/>
+      <c r="A51" s="71"/>
       <c r="B51" s="21">
         <v>3.472222222222222E-3</v>
       </c>
@@ -1772,7 +1812,7 @@
       <c r="E51" s="13"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="48"/>
+      <c r="A52" s="71"/>
       <c r="B52" s="21">
         <v>3.4722222222222224E-2</v>
       </c>
@@ -1783,7 +1823,7 @@
       <c r="E52" s="13"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="48"/>
+      <c r="A53" s="71"/>
       <c r="B53" s="21">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1791,12 +1831,12 @@
         <v>64</v>
       </c>
       <c r="D53" s="16"/>
-      <c r="E53" s="57" t="s">
+      <c r="E53" s="74" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="49"/>
+      <c r="A54" s="68"/>
       <c r="B54" s="21">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1804,10 +1844,10 @@
         <v>66</v>
       </c>
       <c r="D54" s="16"/>
-      <c r="E54" s="57"/>
+      <c r="E54" s="74"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="47">
+      <c r="A55" s="70">
         <v>43378</v>
       </c>
       <c r="B55" s="21"/>
@@ -1816,35 +1856,35 @@
       <c r="E55" s="29"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="48"/>
+      <c r="A56" s="71"/>
       <c r="B56" s="21"/>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
       <c r="E56" s="29"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="48"/>
+      <c r="A57" s="71"/>
       <c r="B57" s="21"/>
       <c r="C57" s="16"/>
       <c r="D57" s="16"/>
       <c r="E57" s="29"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="48"/>
+      <c r="A58" s="71"/>
       <c r="B58" s="21"/>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
       <c r="E58" s="29"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="48"/>
+      <c r="A59" s="71"/>
       <c r="B59" s="21"/>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
       <c r="E59" s="29"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="48"/>
+      <c r="A60" s="71"/>
       <c r="B60" s="21"/>
       <c r="C60" s="16"/>
       <c r="D60" s="16"/>
@@ -1858,12 +1898,12 @@
         <f>SUM(B62:B71)</f>
         <v>0.12847222222222224</v>
       </c>
-      <c r="C61" s="54"/>
-      <c r="D61" s="55"/>
-      <c r="E61" s="56"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="59"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="64">
+      <c r="A62" s="72">
         <v>43382</v>
       </c>
       <c r="B62" s="21">
@@ -1876,7 +1916,7 @@
       <c r="E62" s="13"/>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="48"/>
+      <c r="A63" s="71"/>
       <c r="B63" s="21">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1887,7 +1927,7 @@
       <c r="E63" s="13"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="48"/>
+      <c r="A64" s="71"/>
       <c r="B64" s="21">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -1898,7 +1938,7 @@
       <c r="E64" s="13"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="48"/>
+      <c r="A65" s="71"/>
       <c r="B65" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -1909,7 +1949,7 @@
       <c r="E65" s="13"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="49"/>
+      <c r="A66" s="68"/>
       <c r="B66" s="21">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -1922,7 +1962,7 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="47">
+      <c r="A67" s="70">
         <v>43385</v>
       </c>
       <c r="B67" s="35">
@@ -1937,7 +1977,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="48"/>
+      <c r="A68" s="71"/>
       <c r="B68" s="38">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1948,21 +1988,21 @@
       <c r="E68" s="40"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="48"/>
+      <c r="A69" s="71"/>
       <c r="B69" s="39"/>
       <c r="C69" s="39"/>
       <c r="D69" s="39"/>
       <c r="E69" s="40"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="48"/>
+      <c r="A70" s="71"/>
       <c r="B70" s="39"/>
       <c r="C70" s="39"/>
       <c r="D70" s="39"/>
       <c r="E70" s="40"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="49"/>
+      <c r="A71" s="68"/>
       <c r="B71" s="41"/>
       <c r="C71" s="41"/>
       <c r="D71" s="41"/>
@@ -1972,75 +2012,75 @@
       <c r="A72" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="C72" s="52" t="s">
+      <c r="C72" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="D72" s="52"/>
-      <c r="E72" s="53"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="61"/>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="65" t="s">
+      <c r="A73" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="66">
-        <f>SUM(B74:B85)</f>
+      <c r="B73" s="51">
+        <f>SUM(B74:B83)</f>
         <v>0.1736111111111111</v>
       </c>
-      <c r="C73" s="54"/>
-      <c r="D73" s="55"/>
-      <c r="E73" s="56"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="49"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="43">
+      <c r="A74" s="44">
         <v>43404</v>
       </c>
       <c r="B74" s="21">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C74" s="67" t="s">
+      <c r="C74" s="52" t="s">
         <v>86</v>
       </c>
       <c r="D74" s="36"/>
       <c r="E74" s="37"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="44"/>
+      <c r="A75" s="45"/>
       <c r="C75" s="16"/>
       <c r="D75" s="16"/>
-      <c r="E75" s="68"/>
+      <c r="E75" s="53"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="44"/>
+      <c r="A76" s="45"/>
       <c r="B76" s="21"/>
       <c r="C76" s="16"/>
       <c r="D76" s="16"/>
-      <c r="E76" s="68"/>
+      <c r="E76" s="53"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="44"/>
+      <c r="A77" s="45"/>
       <c r="B77" s="21"/>
       <c r="C77" s="16"/>
       <c r="D77" s="16"/>
-      <c r="E77" s="68"/>
+      <c r="E77" s="53"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="45"/>
-      <c r="B78" s="69"/>
-      <c r="C78" s="70"/>
-      <c r="D78" s="70"/>
-      <c r="E78" s="71"/>
+      <c r="A78" s="46"/>
+      <c r="B78" s="54"/>
+      <c r="C78" s="55"/>
+      <c r="D78" s="55"/>
+      <c r="E78" s="56"/>
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="43">
-        <v>43375</v>
+      <c r="A79" s="44">
+        <v>43406</v>
       </c>
       <c r="B79" s="35">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="C79" s="67" t="s">
+      <c r="C79" s="52" t="s">
         <v>87</v>
       </c>
       <c r="D79" s="36"/>
@@ -2049,7 +2089,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="44"/>
+      <c r="A80" s="45"/>
       <c r="B80" s="21">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -2057,84 +2097,130 @@
         <v>85</v>
       </c>
       <c r="D80" s="16"/>
-      <c r="E80" s="68" t="s">
+      <c r="E80" s="53" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="44"/>
+      <c r="A81" s="45"/>
       <c r="B81" s="21">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="C81" s="16"/>
+      <c r="C81" t="s">
+        <v>91</v>
+      </c>
       <c r="D81" s="16"/>
-      <c r="E81" s="68"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="44"/>
+      <c r="E81" s="53"/>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="45"/>
       <c r="B82" s="21">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C82" s="16"/>
+      <c r="C82" s="34" t="s">
+        <v>93</v>
+      </c>
       <c r="D82" s="16"/>
-      <c r="E82" s="68"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="45"/>
-      <c r="B83" s="69">
+      <c r="E82" s="53"/>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="46"/>
+      <c r="B83" s="54">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="C83" s="70"/>
-      <c r="D83" s="70"/>
-      <c r="E83" s="71"/>
+      <c r="C83" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="D83" s="55"/>
+      <c r="E83" s="56"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84"/>
-      <c r="B84"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85"/>
-      <c r="B85"/>
+      <c r="A84" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="51">
+        <f>SUM(B86:B90)</f>
+        <v>3.8194444444444448E-2</v>
+      </c>
+      <c r="C84" s="47"/>
+      <c r="D84" s="48"/>
+      <c r="E84" s="49"/>
+    </row>
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="75">
+        <v>43410</v>
+      </c>
+      <c r="B85" s="76">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C85" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="D85" s="78"/>
+      <c r="E85" s="78"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86"/>
-      <c r="B86"/>
+      <c r="A86" s="79"/>
+      <c r="B86" s="76">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="C86" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D86" s="78"/>
+      <c r="E86" s="78"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87"/>
-      <c r="B87"/>
+      <c r="A87" s="79"/>
+      <c r="B87" s="76">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C87" s="79" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" s="78"/>
+      <c r="E87" s="78"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88"/>
-      <c r="B88"/>
+      <c r="A88" s="79"/>
+      <c r="B88" s="79"/>
+      <c r="C88" s="79"/>
+      <c r="D88" s="78"/>
+      <c r="E88" s="78"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89"/>
-      <c r="B89"/>
+      <c r="A89" s="79"/>
+      <c r="B89" s="79"/>
+      <c r="C89" s="79"/>
+      <c r="D89" s="78"/>
+      <c r="E89" s="78"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90"/>
-      <c r="B90"/>
+      <c r="A90" s="79"/>
+      <c r="B90" s="79"/>
+      <c r="C90" s="79"/>
+      <c r="D90" s="78"/>
+      <c r="E90" s="78"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91"/>
-      <c r="B91"/>
+      <c r="A91" s="26"/>
+      <c r="C91" s="26"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92"/>
-      <c r="B92"/>
+      <c r="A92" s="26"/>
+      <c r="C92" s="26"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93"/>
-      <c r="B93"/>
+      <c r="A93" s="26"/>
+      <c r="C93" s="26"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94"/>
-      <c r="B94"/>
+      <c r="A94" s="26"/>
+      <c r="C94" s="26"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95"/>
-      <c r="B95"/>
+      <c r="A95" s="26"/>
+      <c r="C95" s="26"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96"/>
@@ -2241,8 +2327,15 @@
       <c r="B121"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="C73:E73"/>
+  <mergeCells count="23">
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C72:E72"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="A1:C2"/>
@@ -2258,14 +2351,6 @@
     <mergeCell ref="E27:E29"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="E31:E33"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="A37:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>